<commit_message>
Adding percent differences for labs 7-9
</commit_message>
<xml_diff>
--- a/07_starvation/starvation_data.xlsx
+++ b/07_starvation/starvation_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="26">
   <si>
     <t>Time</t>
   </si>
@@ -91,13 +91,16 @@
   </si>
   <si>
     <t>HumMod Starvation Lab</t>
+  </si>
+  <si>
+    <t>% Difference</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,6 +113,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -192,10 +202,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -217,6 +228,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -234,11 +251,56 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -528,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:T15"/>
+  <dimension ref="A2:AD15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="X5" sqref="X5:AD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -539,19 +601,22 @@
     <col min="1" max="1" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:20" ht="15.75" thickBot="1">
+    <row r="2" spans="1:30" ht="15.75" thickBot="1">
       <c r="A2" t="s">
         <v>23</v>
       </c>
       <c r="L2" t="s">
         <v>24</v>
       </c>
+      <c r="W2" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="1:20" ht="15.75" thickBot="1">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:30" ht="15.75" thickBot="1">
+      <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="11">
         <v>0</v>
       </c>
       <c r="C3" s="1">
@@ -575,10 +640,10 @@
       <c r="I3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="M3" s="12">
+      <c r="M3" s="14">
         <v>0</v>
       </c>
       <c r="N3" s="4">
@@ -602,10 +667,34 @@
       <c r="T3" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="W3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="X3" s="11">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="8">
+        <v>6</v>
+      </c>
+      <c r="Z3" s="8">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="8">
+        <v>2</v>
+      </c>
+      <c r="AB3" s="8">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="8">
+        <v>2</v>
+      </c>
+      <c r="AD3" s="8">
+        <v>3</v>
+      </c>
     </row>
-    <row r="4" spans="1:20" ht="15.75" thickBot="1">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9"/>
+    <row r="4" spans="1:30" ht="15.75" thickBot="1">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
@@ -625,8 +714,8 @@
         <v>5</v>
       </c>
       <c r="I4" s="2"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="15"/>
       <c r="N4" s="5" t="s">
         <v>1</v>
       </c>
@@ -646,8 +735,28 @@
         <v>5</v>
       </c>
       <c r="T4" s="2"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="11"/>
+      <c r="Y4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD4" s="8" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="5" spans="1:20" ht="45.75" thickBot="1">
+    <row r="5" spans="1:30" ht="45.75" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -702,8 +811,39 @@
       <c r="T5" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="W5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="X5" s="16">
+        <f>ABS((B5-M5)/B5)</f>
+        <v>0.13700000000000004</v>
+      </c>
+      <c r="Y5" s="16">
+        <f t="shared" ref="Y5:AD5" si="0">ABS((C5-N5)/C5)</f>
+        <v>0.23380281690140836</v>
+      </c>
+      <c r="Z5" s="16">
+        <f t="shared" si="0"/>
+        <v>0.16818181818181815</v>
+      </c>
+      <c r="AA5" s="16">
+        <f t="shared" si="0"/>
+        <v>0.36153846153846148</v>
+      </c>
+      <c r="AB5" s="16">
+        <f t="shared" si="0"/>
+        <v>0.86363636363636365</v>
+      </c>
+      <c r="AC5" s="16">
+        <f t="shared" si="0"/>
+        <v>0.94000000000000006</v>
+      </c>
+      <c r="AD5" s="16">
+        <f t="shared" si="0"/>
+        <v>0.93333333333333324</v>
+      </c>
     </row>
-    <row r="6" spans="1:20" ht="30.75" thickBot="1">
+    <row r="6" spans="1:30" ht="30.75" thickBot="1">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -758,8 +898,39 @@
       <c r="T6" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="W6" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="X6" s="16">
+        <f t="shared" ref="X6:X15" si="1">ABS((B6-M6)/B6)</f>
+        <v>0.17997033935269999</v>
+      </c>
+      <c r="Y6" s="16">
+        <f t="shared" ref="Y6:Y15" si="2">ABS((C6-N6)/C6)</f>
+        <v>0.18016601135867191</v>
+      </c>
+      <c r="Z6" s="16">
+        <f t="shared" ref="Z6:Z15" si="3">ABS((D6-O6)/D6)</f>
+        <v>0.18177813023173847</v>
+      </c>
+      <c r="AA6" s="16">
+        <f t="shared" ref="AA6:AA15" si="4">ABS((E6-P6)/E6)</f>
+        <v>0.18464563410492449</v>
+      </c>
+      <c r="AB6" s="16">
+        <f t="shared" ref="AB6:AB15" si="5">ABS((F6-Q6)/F6)</f>
+        <v>0.20354410767889997</v>
+      </c>
+      <c r="AC6" s="16">
+        <f t="shared" ref="AC6:AC15" si="6">ABS((G6-R6)/G6)</f>
+        <v>0.22196595277320152</v>
+      </c>
+      <c r="AD6" s="16">
+        <f t="shared" ref="AD6:AD15" si="7">ABS((H6-S6)/H6)</f>
+        <v>0.23884152457372115</v>
+      </c>
     </row>
-    <row r="7" spans="1:20" ht="30.75" thickBot="1">
+    <row r="7" spans="1:30" ht="30.75" thickBot="1">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -814,8 +985,39 @@
       <c r="T7" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="W7" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="X7" s="16">
+        <f t="shared" si="1"/>
+        <v>2.9538665781613009E-2</v>
+      </c>
+      <c r="Y7" s="16">
+        <f t="shared" si="2"/>
+        <v>2.8990336554481841E-2</v>
+      </c>
+      <c r="Z7" s="16">
+        <f t="shared" si="3"/>
+        <v>2.6395939086294416E-2</v>
+      </c>
+      <c r="AA7" s="16">
+        <f t="shared" si="4"/>
+        <v>2.4213075060532687E-2</v>
+      </c>
+      <c r="AB7" s="16">
+        <f t="shared" si="5"/>
+        <v>3.4188034188034191E-2</v>
+      </c>
+      <c r="AC7" s="16">
+        <f t="shared" si="6"/>
+        <v>5.2164502164502163E-2</v>
+      </c>
+      <c r="AD7" s="16">
+        <f t="shared" si="7"/>
+        <v>3.4534913032518273E-2</v>
+      </c>
     </row>
-    <row r="8" spans="1:20" ht="30.75" thickBot="1">
+    <row r="8" spans="1:30" ht="30.75" thickBot="1">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -870,8 +1072,39 @@
       <c r="T8" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="W8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="X8" s="16">
+        <f t="shared" si="1"/>
+        <v>6.2499999999999982</v>
+      </c>
+      <c r="Y8" s="16">
+        <f t="shared" si="2"/>
+        <v>3.5135135135135132</v>
+      </c>
+      <c r="Z8" s="16">
+        <f t="shared" si="3"/>
+        <v>5.0076335877862599</v>
+      </c>
+      <c r="AA8" s="16">
+        <f t="shared" si="4"/>
+        <v>2.5216095380029802</v>
+      </c>
+      <c r="AB8" s="16">
+        <f t="shared" si="5"/>
+        <v>1.9894117647058824</v>
+      </c>
+      <c r="AC8" s="16">
+        <f t="shared" si="6"/>
+        <v>0.62665310274669384</v>
+      </c>
+      <c r="AD8" s="16">
+        <f t="shared" si="7"/>
+        <v>0.69691780821917815</v>
+      </c>
     </row>
-    <row r="9" spans="1:20" ht="30.75" thickBot="1">
+    <row r="9" spans="1:30" ht="30.75" thickBot="1">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -926,8 +1159,39 @@
       <c r="T9" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="W9" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="X9" s="16">
+        <f t="shared" si="1"/>
+        <v>5.8878504672897167E-2</v>
+      </c>
+      <c r="Y9" s="16">
+        <f t="shared" si="2"/>
+        <v>7.85714285714285E-2</v>
+      </c>
+      <c r="Z9" s="16">
+        <f t="shared" si="3"/>
+        <v>7.3684210526315838E-2</v>
+      </c>
+      <c r="AA9" s="16">
+        <f t="shared" si="4"/>
+        <v>0.22830188679245286</v>
+      </c>
+      <c r="AB9" s="16">
+        <f t="shared" si="5"/>
+        <v>0.25510204081632654</v>
+      </c>
+      <c r="AC9" s="16">
+        <f t="shared" si="6"/>
+        <v>0.83400000000000007</v>
+      </c>
+      <c r="AD9" s="16">
+        <f t="shared" si="7"/>
+        <v>0.90204081632653066</v>
+      </c>
     </row>
-    <row r="10" spans="1:20" ht="30.75" thickBot="1">
+    <row r="10" spans="1:30" ht="30.75" thickBot="1">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
@@ -982,8 +1246,39 @@
       <c r="T10" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="W10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="X10" s="16">
+        <f t="shared" si="1"/>
+        <v>0.73636363636363611</v>
+      </c>
+      <c r="Y10" s="16">
+        <f t="shared" si="2"/>
+        <v>0.18000000000000002</v>
+      </c>
+      <c r="Z10" s="16">
+        <f t="shared" si="3"/>
+        <v>0.76037735849056609</v>
+      </c>
+      <c r="AA10" s="16">
+        <f t="shared" si="4"/>
+        <v>0.20813397129186595</v>
+      </c>
+      <c r="AB10" s="16">
+        <f t="shared" si="5"/>
+        <v>0.25215517241379304</v>
+      </c>
+      <c r="AC10" s="16">
+        <f t="shared" si="6"/>
+        <v>0.19792531120331963</v>
+      </c>
+      <c r="AD10" s="16">
+        <f t="shared" si="7"/>
+        <v>0.49473684210526314</v>
+      </c>
     </row>
-    <row r="11" spans="1:20" ht="30.75" thickBot="1">
+    <row r="11" spans="1:30" ht="30.75" thickBot="1">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
@@ -1038,8 +1333,39 @@
       <c r="T11" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="W11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="X11" s="16">
+        <f t="shared" si="1"/>
+        <v>0.15124555160142347</v>
+      </c>
+      <c r="Y11" s="16">
+        <f t="shared" si="2"/>
+        <v>0.12972972972972979</v>
+      </c>
+      <c r="Z11" s="16">
+        <f t="shared" si="3"/>
+        <v>0.32112068965517238</v>
+      </c>
+      <c r="AA11" s="16">
+        <f t="shared" si="4"/>
+        <v>0.33333333333333337</v>
+      </c>
+      <c r="AB11" s="16">
+        <f t="shared" si="5"/>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="AC11" s="16">
+        <f t="shared" si="6"/>
+        <v>0.36645962732919241</v>
+      </c>
+      <c r="AD11" s="16">
+        <f t="shared" si="7"/>
+        <v>0.60269360269360261</v>
+      </c>
     </row>
-    <row r="12" spans="1:20" ht="30.75" thickBot="1">
+    <row r="12" spans="1:30" ht="30.75" thickBot="1">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -1094,8 +1420,39 @@
       <c r="T12" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="W12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="X12" s="16">
+        <f t="shared" si="1"/>
+        <v>0.22368421052631571</v>
+      </c>
+      <c r="Y12" s="16">
+        <f t="shared" si="2"/>
+        <v>0.31372549019607854</v>
+      </c>
+      <c r="Z12" s="16">
+        <f t="shared" si="3"/>
+        <v>0.23333333333333339</v>
+      </c>
+      <c r="AA12" s="16">
+        <f t="shared" si="4"/>
+        <v>0.36842105263157904</v>
+      </c>
+      <c r="AB12" s="16">
+        <f t="shared" si="5"/>
+        <v>0.16666666666666669</v>
+      </c>
+      <c r="AC12" s="16">
+        <f t="shared" si="6"/>
+        <v>0.68421052631578938</v>
+      </c>
+      <c r="AD12" s="16">
+        <f t="shared" si="7"/>
+        <v>0.85714285714285721</v>
+      </c>
     </row>
-    <row r="13" spans="1:20" ht="45.75" thickBot="1">
+    <row r="13" spans="1:30" ht="45.75" thickBot="1">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
@@ -1150,8 +1507,39 @@
       <c r="T13" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="W13" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="X13" s="16">
+        <f t="shared" si="1"/>
+        <v>0.19200000000000003</v>
+      </c>
+      <c r="Y13" s="16">
+        <f t="shared" si="2"/>
+        <v>0.13970588235294121</v>
+      </c>
+      <c r="Z13" s="16">
+        <f t="shared" si="3"/>
+        <v>6.8965517241379309E-2</v>
+      </c>
+      <c r="AA13" s="16">
+        <f t="shared" si="4"/>
+        <v>6.6666666666666428E-3</v>
+      </c>
+      <c r="AB13" s="16">
+        <f t="shared" si="5"/>
+        <v>0.14569536423841067</v>
+      </c>
+      <c r="AC13" s="16">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="AD13" s="16">
+        <f t="shared" si="7"/>
+        <v>0.23448275862068957</v>
+      </c>
     </row>
-    <row r="14" spans="1:20" ht="15.75" thickBot="1">
+    <row r="14" spans="1:30" ht="15.75" thickBot="1">
       <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
@@ -1206,8 +1594,39 @@
       <c r="T14" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="W14" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="X14" s="16">
+        <f t="shared" si="1"/>
+        <v>9.7087378640776344E-3</v>
+      </c>
+      <c r="Y14" s="16">
+        <f t="shared" si="2"/>
+        <v>0.39259259259259266</v>
+      </c>
+      <c r="Z14" s="16">
+        <f t="shared" si="3"/>
+        <v>0.73529411764705899</v>
+      </c>
+      <c r="AA14" s="16">
+        <f t="shared" si="4"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="AB14" s="16">
+        <f t="shared" si="5"/>
+        <v>0.4499999999999999</v>
+      </c>
+      <c r="AC14" s="16">
+        <f t="shared" si="6"/>
+        <v>0.94736842105263164</v>
+      </c>
+      <c r="AD14" s="16">
+        <f t="shared" si="7"/>
+        <v>0.94736842105263153</v>
+      </c>
     </row>
-    <row r="15" spans="1:20" ht="30.75" thickBot="1">
+    <row r="15" spans="1:30" ht="30.75" thickBot="1">
       <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
@@ -1262,14 +1681,56 @@
       <c r="T15" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="W15" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="X15" s="16">
+        <f t="shared" si="1"/>
+        <v>0.10649350649350653</v>
+      </c>
+      <c r="Y15" s="16">
+        <f t="shared" si="2"/>
+        <v>0.21868131868131874</v>
+      </c>
+      <c r="Z15" s="16">
+        <f t="shared" si="3"/>
+        <v>0.14921874999999996</v>
+      </c>
+      <c r="AA15" s="16">
+        <f t="shared" si="4"/>
+        <v>0.18538011695906426</v>
+      </c>
+      <c r="AB15" s="16">
+        <f t="shared" si="5"/>
+        <v>0.18835978835978834</v>
+      </c>
+      <c r="AC15" s="16">
+        <f t="shared" si="6"/>
+        <v>4.4042682926829269</v>
+      </c>
+      <c r="AD15" s="16">
+        <f t="shared" si="7"/>
+        <v>1.7699421965317919</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="X3:X4"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="L3:L4"/>
     <mergeCell ref="M3:M4"/>
+    <mergeCell ref="W3:W4"/>
   </mergeCells>
+  <conditionalFormatting sqref="X5:AD15">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="between">
+      <formula>0.5</formula>
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixing Lab 7 charts
</commit_message>
<xml_diff>
--- a/07_starvation/starvation_data.xlsx
+++ b/07_starvation/starvation_data.xlsx
@@ -228,16 +228,16 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -251,45 +251,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -592,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:AD15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="X5" sqref="X5:AD15"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="AE7" sqref="AE7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -613,10 +585,10 @@
       </c>
     </row>
     <row r="3" spans="1:30" ht="15.75" thickBot="1">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="10">
         <v>0</v>
       </c>
       <c r="C3" s="1">
@@ -667,34 +639,34 @@
       <c r="T3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="W3" s="10" t="s">
+      <c r="W3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="X3" s="11">
+      <c r="X3" s="10">
         <v>0</v>
       </c>
-      <c r="Y3" s="8">
+      <c r="Y3" s="9">
         <v>6</v>
       </c>
-      <c r="Z3" s="8">
+      <c r="Z3" s="9">
         <v>1</v>
       </c>
-      <c r="AA3" s="8">
+      <c r="AA3" s="9">
         <v>2</v>
       </c>
-      <c r="AB3" s="8">
+      <c r="AB3" s="9">
         <v>1</v>
       </c>
-      <c r="AC3" s="8">
+      <c r="AC3" s="9">
         <v>2</v>
       </c>
-      <c r="AD3" s="8">
+      <c r="AD3" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:30" ht="15.75" thickBot="1">
-      <c r="A4" s="10"/>
-      <c r="B4" s="11"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="10"/>
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
@@ -735,24 +707,24 @@
         <v>5</v>
       </c>
       <c r="T4" s="2"/>
-      <c r="W4" s="10"/>
-      <c r="X4" s="11"/>
-      <c r="Y4" s="8" t="s">
+      <c r="W4" s="11"/>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="Z4" s="8" t="s">
+      <c r="Z4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="AA4" s="8" t="s">
+      <c r="AA4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="AB4" s="8" t="s">
+      <c r="AB4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="AC4" s="8" t="s">
+      <c r="AC4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="AD4" s="8" t="s">
+      <c r="AD4" s="9" t="s">
         <v>5</v>
       </c>
     </row>
@@ -811,7 +783,7 @@
       <c r="T5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="W5" s="9" t="s">
+      <c r="W5" s="8" t="s">
         <v>6</v>
       </c>
       <c r="X5" s="16">
@@ -898,7 +870,7 @@
       <c r="T6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="W6" s="9" t="s">
+      <c r="W6" s="8" t="s">
         <v>7</v>
       </c>
       <c r="X6" s="16">
@@ -985,7 +957,7 @@
       <c r="T7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="W7" s="9" t="s">
+      <c r="W7" s="8" t="s">
         <v>8</v>
       </c>
       <c r="X7" s="16">
@@ -1072,7 +1044,7 @@
       <c r="T8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="W8" s="9" t="s">
+      <c r="W8" s="8" t="s">
         <v>9</v>
       </c>
       <c r="X8" s="16">
@@ -1159,7 +1131,7 @@
       <c r="T9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="W9" s="9" t="s">
+      <c r="W9" s="8" t="s">
         <v>10</v>
       </c>
       <c r="X9" s="16">
@@ -1246,7 +1218,7 @@
       <c r="T10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="W10" s="9" t="s">
+      <c r="W10" s="8" t="s">
         <v>11</v>
       </c>
       <c r="X10" s="16">
@@ -1333,7 +1305,7 @@
       <c r="T11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="W11" s="9" t="s">
+      <c r="W11" s="8" t="s">
         <v>12</v>
       </c>
       <c r="X11" s="16">
@@ -1420,7 +1392,7 @@
       <c r="T12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="W12" s="9" t="s">
+      <c r="W12" s="8" t="s">
         <v>13</v>
       </c>
       <c r="X12" s="16">
@@ -1507,7 +1479,7 @@
       <c r="T13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="W13" s="9" t="s">
+      <c r="W13" s="8" t="s">
         <v>14</v>
       </c>
       <c r="X13" s="16">
@@ -1594,7 +1566,7 @@
       <c r="T14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W14" s="9" t="s">
+      <c r="W14" s="8" t="s">
         <v>15</v>
       </c>
       <c r="X14" s="16">
@@ -1681,7 +1653,7 @@
       <c r="T15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="W15" s="9" t="s">
+      <c r="W15" s="8" t="s">
         <v>16</v>
       </c>
       <c r="X15" s="16">
@@ -1723,11 +1695,11 @@
     <mergeCell ref="W3:W4"/>
   </mergeCells>
   <conditionalFormatting sqref="X5:AD15">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
       <formula>0.5</formula>
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>